<commit_message>
changes to heuristicai2 according to AI lecture
</commit_message>
<xml_diff>
--- a/P02_2048/Auswertung_AITypen.xlsx
+++ b/P02_2048/Auswertung_AITypen.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEC\Documents\GitHub\HS2017_KI1\P02_2048\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claude\Documents\ZHAW\Semester 5\KI1\HS2017_KI1\P02_2048\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle5" sheetId="5" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabelle4" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_20171012_225832_heuristicai2_totals" localSheetId="0">Tabelle2!$B$6:$C$55</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Type</t>
   </si>
@@ -94,6 +95,30 @@
   </si>
   <si>
     <t>Häufigkeit</t>
+  </si>
+  <si>
+    <t>4k</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>ndh</t>
+  </si>
+  <si>
+    <t>ecc</t>
+  </si>
+  <si>
+    <t>htic</t>
+  </si>
+  <si>
+    <t>heuristic</t>
   </si>
 </sst>
 </file>
@@ -156,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -217,6 +248,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -355,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="624970512"/>
-        <c:axId val="620804656"/>
+        <c:axId val="-1117532416"/>
+        <c:axId val="-1117536224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="624970512"/>
+        <c:axId val="-1117532416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,12 +420,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="620804656"/>
+        <c:crossAx val="-1117536224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="620804656"/>
+        <c:axId val="-1117536224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,7 +454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624970512"/>
+        <c:crossAx val="-1117532416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1125,11 +1157,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="423504016"/>
-        <c:axId val="423515216"/>
+        <c:axId val="-1117534048"/>
+        <c:axId val="-1117536768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="423504016"/>
+        <c:axId val="-1117534048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1172,7 +1204,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423515216"/>
+        <c:crossAx val="-1117536768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1180,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423515216"/>
+        <c:axId val="-1117536768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1263,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423504016"/>
+        <c:crossAx val="-1117534048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1971,11 +2003,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="423509056"/>
-        <c:axId val="423506256"/>
+        <c:axId val="-1117535136"/>
+        <c:axId val="-1117533504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="423509056"/>
+        <c:axId val="-1117535136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2018,7 +2050,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423506256"/>
+        <c:crossAx val="-1117533504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2026,7 +2058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423506256"/>
+        <c:axId val="-1117533504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2077,7 +2109,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423509056"/>
+        <c:crossAx val="-1117535136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3614,17 +3646,17 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" customWidth="1"/>
+    <col min="2" max="2" width="11.1328125" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3635,7 +3667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3648,7 +3680,7 @@
         <v>385.28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3661,7 +3693,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3674,7 +3706,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>7012</v>
       </c>
@@ -3682,7 +3714,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>6516</v>
       </c>
@@ -3690,7 +3722,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>5492</v>
       </c>
@@ -3698,7 +3730,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>13220</v>
       </c>
@@ -3706,7 +3738,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>6980</v>
       </c>
@@ -3714,7 +3746,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>3172</v>
       </c>
@@ -3722,7 +3754,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>3220</v>
       </c>
@@ -3730,7 +3762,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>3828</v>
       </c>
@@ -3738,7 +3770,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>4820</v>
       </c>
@@ -3746,7 +3778,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>6292</v>
       </c>
@@ -3754,7 +3786,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>1716</v>
       </c>
@@ -3762,7 +3794,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>6348</v>
       </c>
@@ -3770,7 +3802,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>14360</v>
       </c>
@@ -3778,7 +3810,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>7284</v>
       </c>
@@ -3786,7 +3818,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>1776</v>
       </c>
@@ -3794,7 +3826,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>10764</v>
       </c>
@@ -3802,7 +3834,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>3080</v>
       </c>
@@ -3810,7 +3842,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>4228</v>
       </c>
@@ -3818,7 +3850,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>2960</v>
       </c>
@@ -3826,7 +3858,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>3312</v>
       </c>
@@ -3834,7 +3866,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>5420</v>
       </c>
@@ -3842,7 +3874,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>3244</v>
       </c>
@@ -3850,7 +3882,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>7232</v>
       </c>
@@ -3858,7 +3890,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>2268</v>
       </c>
@@ -3866,7 +3898,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>3068</v>
       </c>
@@ -3874,7 +3906,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>4160</v>
       </c>
@@ -3882,7 +3914,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>4892</v>
       </c>
@@ -3890,7 +3922,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>2368</v>
       </c>
@@ -3898,7 +3930,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>1904</v>
       </c>
@@ -3906,7 +3938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>5584</v>
       </c>
@@ -3914,7 +3946,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>7076</v>
       </c>
@@ -3922,7 +3954,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>10584</v>
       </c>
@@ -3930,7 +3962,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>3004</v>
       </c>
@@ -3938,7 +3970,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>12504</v>
       </c>
@@ -3946,7 +3978,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>4076</v>
       </c>
@@ -3954,7 +3986,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>856</v>
       </c>
@@ -3962,7 +3994,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>2440</v>
       </c>
@@ -3970,7 +4002,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>3192</v>
       </c>
@@ -3978,7 +4010,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>3144</v>
       </c>
@@ -3986,7 +4018,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>2272</v>
       </c>
@@ -3994,7 +4026,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>6144</v>
       </c>
@@ -4002,7 +4034,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>1052</v>
       </c>
@@ -4010,7 +4042,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>7248</v>
       </c>
@@ -4018,7 +4050,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>6476</v>
       </c>
@@ -4026,7 +4058,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>5748</v>
       </c>
@@ -4034,7 +4066,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>2408</v>
       </c>
@@ -4042,7 +4074,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>3264</v>
       </c>
@@ -4050,7 +4082,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>5260</v>
       </c>
@@ -4058,7 +4090,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>3184</v>
       </c>
@@ -4066,7 +4098,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>3964</v>
       </c>
@@ -4083,13 +4115,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
@@ -4097,7 +4129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="8">
         <v>1000</v>
       </c>
@@ -4105,7 +4137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="8">
         <v>3080.5714285714284</v>
       </c>
@@ -4113,7 +4145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="8">
         <v>5161.1428571428569</v>
       </c>
@@ -4121,7 +4153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="8">
         <v>7241.7142857142853</v>
       </c>
@@ -4129,7 +4161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="8">
         <v>9322.2857142857138</v>
       </c>
@@ -4137,7 +4169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="8">
         <v>11402.857142857141</v>
       </c>
@@ -4145,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="8">
         <v>13483.428571428571</v>
       </c>
@@ -4153,7 +4185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -4171,13 +4203,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4188,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -4201,7 +4233,7 @@
         <v>474.88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4214,7 +4246,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4227,7 +4259,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1000</v>
       </c>
@@ -4235,7 +4267,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1972</v>
       </c>
@@ -4243,7 +4275,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>2088</v>
       </c>
@@ -4251,7 +4283,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>2200</v>
       </c>
@@ -4259,7 +4291,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>2420</v>
       </c>
@@ -4267,7 +4299,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>2904</v>
       </c>
@@ -4275,7 +4307,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>3040</v>
       </c>
@@ -4283,7 +4315,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>3084</v>
       </c>
@@ -4291,7 +4323,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>3112</v>
       </c>
@@ -4299,7 +4331,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>3120</v>
       </c>
@@ -4307,7 +4339,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>3180</v>
       </c>
@@ -4315,7 +4347,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>3180</v>
       </c>
@@ -4323,7 +4355,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>3236</v>
       </c>
@@ -4331,7 +4363,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>3236</v>
       </c>
@@ -4339,7 +4371,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>3356</v>
       </c>
@@ -4347,7 +4379,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>3432</v>
       </c>
@@ -4355,7 +4387,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>3564</v>
       </c>
@@ -4363,7 +4395,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>3696</v>
       </c>
@@ -4371,7 +4403,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>3868</v>
       </c>
@@ -4379,7 +4411,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>3924</v>
       </c>
@@ -4387,7 +4419,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>4232</v>
       </c>
@@ -4395,7 +4427,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>4268</v>
       </c>
@@ -4403,7 +4435,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>4340</v>
       </c>
@@ -4411,7 +4443,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>4648</v>
       </c>
@@ -4419,7 +4451,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>4900</v>
       </c>
@@ -4427,7 +4459,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>5324</v>
       </c>
@@ -4435,7 +4467,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>5440</v>
       </c>
@@ -4443,7 +4475,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>5464</v>
       </c>
@@ -4451,7 +4483,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>5628</v>
       </c>
@@ -4459,7 +4491,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>6232</v>
       </c>
@@ -4467,7 +4499,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>6372</v>
       </c>
@@ -4475,7 +4507,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>6376</v>
       </c>
@@ -4483,7 +4515,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>6476</v>
       </c>
@@ -4491,7 +4523,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>6672</v>
       </c>
@@ -4499,7 +4531,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>7068</v>
       </c>
@@ -4507,7 +4539,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>7076</v>
       </c>
@@ -4515,7 +4547,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>7152</v>
       </c>
@@ -4523,7 +4555,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>7192</v>
       </c>
@@ -4531,7 +4563,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>7276</v>
       </c>
@@ -4539,7 +4571,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>10128</v>
       </c>
@@ -4547,7 +4579,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>11420</v>
       </c>
@@ -4555,7 +4587,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>11444</v>
       </c>
@@ -4563,7 +4595,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>12232</v>
       </c>
@@ -4571,7 +4603,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>12264</v>
       </c>
@@ -4579,7 +4611,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>12568</v>
       </c>
@@ -4587,7 +4619,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>12792</v>
       </c>
@@ -4595,7 +4627,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>13956</v>
       </c>
@@ -4603,7 +4635,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>14300</v>
       </c>
@@ -4611,7 +4643,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>14776</v>
       </c>
@@ -4619,7 +4651,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>15564</v>
       </c>
@@ -4639,13 +4671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4671,7 +4703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4697,7 +4729,7 @@
         <v>4216</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4723,7 +4755,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4749,7 +4781,7 @@
         <v>16144</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4775,7 +4807,7 @@
         <v>5596</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4801,7 +4833,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4827,7 +4859,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4853,7 +4885,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4879,7 +4911,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4905,7 +4937,7 @@
         <v>7028</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4928,7 +4960,7 @@
         <v>3176</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -4961,7 +4993,7 @@
         <v>5347.5555555555557</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
@@ -4994,7 +5026,7 @@
         <v>16144</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -5027,40 +5059,40 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="7">
-        <f>B15-B16</f>
+        <f t="shared" ref="B17:H17" si="5">B15-B16</f>
         <v>8700</v>
       </c>
       <c r="C17" s="7">
-        <f>C15-C16</f>
+        <f t="shared" si="5"/>
         <v>2428</v>
       </c>
       <c r="D17" s="7">
-        <f>D15-D16</f>
+        <f t="shared" si="5"/>
         <v>8680</v>
       </c>
       <c r="E17" s="7">
-        <f>E15-E16</f>
+        <f t="shared" si="5"/>
         <v>8852</v>
       </c>
       <c r="F17" s="7">
-        <f>F15-F16</f>
+        <f t="shared" si="5"/>
         <v>10180</v>
       </c>
       <c r="G17" s="7">
-        <f>G15-G16</f>
+        <f t="shared" si="5"/>
         <v>12848</v>
       </c>
       <c r="H17" s="7">
-        <f>H15-H16</f>
+        <f t="shared" si="5"/>
         <v>14700</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -5069,31 +5101,31 @@
         <v>0.79252295583734145</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" ref="C18:H18" si="5">((C17/2)/C14)</f>
+        <f t="shared" ref="C18:H18" si="6">((C17/2)/C14)</f>
         <v>0.45089882632595452</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.74606339819844603</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.60438059864540095</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.93223443223443225</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.000436055565938</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3744597739361701</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -5116,7 +5148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5139,7 +5171,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2</v>
       </c>
@@ -5162,7 +5194,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>3</v>
       </c>
@@ -5185,7 +5217,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>4</v>
       </c>
@@ -5208,7 +5240,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>5</v>
       </c>
@@ -5231,7 +5263,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>6</v>
       </c>
@@ -5254,7 +5286,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>7</v>
       </c>
@@ -5277,7 +5309,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>8</v>
       </c>
@@ -5300,7 +5332,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>9</v>
       </c>
@@ -5323,7 +5355,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>10</v>
       </c>
@@ -5346,7 +5378,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
@@ -5355,27 +5387,27 @@
         <v>460.8</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" ref="C31:G31" si="6">SUM(C21:C30)/10</f>
+        <f t="shared" ref="C31:G31" si="7">SUM(C21:C30)/10</f>
         <v>230.4</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>460.8</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>588.79999999999995</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>422.4</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>524.79999999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -5384,27 +5416,27 @@
         <v>1024</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" ref="C32:G32" si="7">MAX(C21:C30)</f>
+        <f t="shared" ref="C32:G32" si="8">MAX(C21:C30)</f>
         <v>256</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -5413,34 +5445,34 @@
         <v>128</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" ref="C33:G33" si="8">MIN(C21:C30)</f>
+        <f t="shared" ref="C33:G33" si="9">MIN(C21:C30)</f>
         <v>128</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>256</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>256</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F35" s="1"/>
     </row>
   </sheetData>
@@ -5451,4 +5483,167 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E4:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="4" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>64</v>
+      </c>
+      <c r="K5">
+        <v>128</v>
+      </c>
+      <c r="L5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="I6">
+        <v>512</v>
+      </c>
+      <c r="J6">
+        <v>1024</v>
+      </c>
+      <c r="K6">
+        <v>2048</v>
+      </c>
+      <c r="L6">
+        <v>4096</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="I7">
+        <v>8192</v>
+      </c>
+      <c r="J7">
+        <v>16384</v>
+      </c>
+      <c r="K7">
+        <v>32768</v>
+      </c>
+      <c r="L7">
+        <v>65536</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="O13">
+        <v>64</v>
+      </c>
+      <c r="P13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>32</v>
+      </c>
+      <c r="P14">
+        <v>128</v>
+      </c>
+      <c r="Q14">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.45">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>